<commit_message>
Excel Bulk uplod implementation
Excel Bulk uplod implementation
</commit_message>
<xml_diff>
--- a/ShipmentInfo-GoDeliverNCR.xlsx
+++ b/ShipmentInfo-GoDeliverNCR.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\GKCouriers\GIT\mage-bera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Products\CargoTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5822DA-1AB2-4E2E-8708-66C954C6EEAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShipmentInformation" sheetId="1" r:id="rId1"/>
+    <sheet name="Masters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Consignment No</t>
   </si>
@@ -176,36 +178,15 @@
     <t>27-03-2018 12:30</t>
   </si>
   <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Vellore</t>
   </si>
   <si>
-    <t>magesh2522@gmail.com</t>
-  </si>
-  <si>
     <t>No 9 Kothandavar Kovil st Edayansathu Vellore</t>
   </si>
   <si>
-    <t>Pugazhanthi</t>
-  </si>
-  <si>
-    <t>Lodhi Colony Delhi</t>
-  </si>
-  <si>
-    <t>godeliverncr@gmail.com</t>
-  </si>
-  <si>
     <t>Kalaiyarasan G</t>
   </si>
   <si>
-    <t xml:space="preserve"> Magesh K</t>
-  </si>
-  <si>
     <t>kalaiyarasange@gmail.com</t>
   </si>
   <si>
@@ -219,15 +200,42 @@
   </si>
   <si>
     <t>mageshk@bosch.com</t>
+  </si>
+  <si>
+    <t>Consignee Name</t>
+  </si>
+  <si>
+    <t>Consignee Phone No</t>
+  </si>
+  <si>
+    <t>Consignee Address</t>
+  </si>
+  <si>
+    <t>Consignee City</t>
+  </si>
+  <si>
+    <t>Consignee PinCode</t>
+  </si>
+  <si>
+    <t>Consignee EmailId</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>+91 9443776790</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>test18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,26 +356,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -648,113 +689,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AO8"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O2" sqref="O2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="12" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="16" customWidth="1"/>
+    <col min="16" max="16" width="22" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" style="11" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" style="11" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" style="11" customWidth="1"/>
+    <col min="25" max="25" width="7.28515625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="7" style="11" customWidth="1"/>
+    <col min="27" max="27" width="8.42578125" style="12" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="16" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:32" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="11" t="s">
+      <c r="I1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="V1" s="5" t="s">
@@ -772,277 +814,296 @@
       <c r="Z1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:41" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="16">
+        <v>632002</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="16">
+        <v>9629313798</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="16">
+        <v>560068</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="W2" s="11">
+        <v>1.234</v>
+      </c>
+      <c r="AD2" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2">
-        <v>9629313798</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2">
-        <v>632002</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2">
-        <v>9500302626</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2">
-        <v>738384</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AE2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3">
-        <v>9443776790</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3">
-        <v>632002</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3">
-        <v>9629313798</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3">
-        <v>560068</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO3" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AK4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO4" s="9"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AK5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN7" s="9"/>
-      <c r="AO7" s="9"/>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576">
-      <formula1>$AK$2:$AK$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576">
-      <formula1>$AL$2:$AL$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:S1048576">
-      <formula1>$AM$2:$AM$8</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576 U1:U1048576">
-      <formula1>$AN$2:$AN$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="N2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="N3" r:id="rId4"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Masters!$G$2:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q1:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>Masters!$H$2:$H$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>R1:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+          <x14:formula1>
+            <xm:f>Masters!$I$2:$I$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>S1:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+          <x14:formula1>
+            <xm:f>Masters!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>T1:U1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+          <x14:formula1>
+            <xm:f>Masters!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AD1:AD1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
+          <x14:formula1>
+            <xm:f>Masters!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AF1:AF1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="G1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GodeliverNCR ready to move to Production
GodeliverNCR ready to move to Production
</commit_message>
<xml_diff>
--- a/ShipmentInfo-GoDeliverNCR.xlsx
+++ b/ShipmentInfo-GoDeliverNCR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Products\CargoTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5822DA-1AB2-4E2E-8708-66C954C6EEAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B60369-5A70-484E-A5E3-311E8E7BEB0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>FEDEX</t>
   </si>
   <si>
-    <t>25-03-2018 12:30</t>
-  </si>
-  <si>
     <t>27-03-2018 12:30</t>
   </si>
   <si>
@@ -229,7 +226,10 @@
     <t>test123</t>
   </si>
   <si>
-    <t>test18</t>
+    <t>09-06-2019 12:30</t>
+  </si>
+  <si>
+    <t>test24</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,22 +761,22 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="O1" s="15" t="s">
         <v>8</v>
@@ -841,46 +841,46 @@
         <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="16">
         <v>632002</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J2" s="16">
         <v>9629313798</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="16">
         <v>560068</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>26</v>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>46</v>
@@ -1000,7 +1000,7 @@
         <v>25</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="7:12" ht="30" x14ac:dyDescent="0.25">

</xml_diff>